<commit_message>
changed formatting and added formula to generate the python dict entry
</commit_message>
<xml_diff>
--- a/doc/mrange_analysis.xlsx
+++ b/doc/mrange_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u4ul\analises\click\pyclick\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93CC8455-EA88-4601-AEF2-F745DF84336D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E0BC45-066A-4413-968F-1A5DF35663A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{34110A29-B735-4B1F-BA31-255852F7D6AF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="41">
   <si>
     <t>DAY</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>PYTHON</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E20BF456-4668-4AC3-B9A5-0D3A8F1B8082}">
-  <sheetPr codeName="Planilha2"/>
+  <sheetPr codeName="Planilha2" filterMode="1"/>
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="90" workbookViewId="0"/>
@@ -653,6 +656,7 @@
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -686,8 +690,11 @@
       <c r="J1" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K1" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>35</v>
       </c>
@@ -723,7 +730,7 @@
         <v>(True, True, True, True, True, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
@@ -759,7 +766,7 @@
         <v>(True, True, True, True, True, False) : (None, None, None),</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
@@ -831,7 +838,7 @@
         <v>(True, True, True, True, False, False) : (False, False, False),</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>35</v>
       </c>
@@ -867,7 +874,7 @@
         <v>(True, True, True, False, True, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>35</v>
       </c>
@@ -903,7 +910,7 @@
         <v>(True, True, True, False, True, False) : (None, None, None),</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>35</v>
       </c>
@@ -975,7 +982,7 @@
         <v>(True, True, True, False, False, False) : (False, False, True),</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1011,7 +1018,7 @@
         <v>(True, True, False, True, True, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>35</v>
       </c>
@@ -1083,7 +1090,7 @@
         <v>(True, True, False, True, False, True) : (False, False, False),</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>35</v>
       </c>
@@ -1119,7 +1126,7 @@
         <v>(True, True, False, True, False, False) : (None, None, None),</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1155,7 +1162,7 @@
         <v>(True, True, False, False, True, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>35</v>
       </c>
@@ -1263,7 +1270,7 @@
         <v>(True, True, False, False, False, False) : (True, False, False),</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>35</v>
       </c>
@@ -1299,7 +1306,7 @@
         <v>(True, False, True, True, True, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>35</v>
       </c>
@@ -1335,7 +1342,7 @@
         <v>(True, False, True, True, True, False) : (None, None, None),</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>35</v>
       </c>
@@ -1407,7 +1414,7 @@
         <v>(True, False, True, True, False, False) : (False, True, False),</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>35</v>
       </c>
@@ -1443,7 +1450,7 @@
         <v>(True, False, True, False, True, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>35</v>
       </c>
@@ -1479,7 +1486,7 @@
         <v>(True, False, True, False, True, False) : (None, None, None),</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>35</v>
       </c>
@@ -1551,7 +1558,7 @@
         <v>(True, False, True, False, False, False) : (False, True, True),</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
@@ -1587,7 +1594,7 @@
         <v>(True, False, False, True, True, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>35</v>
       </c>
@@ -1659,7 +1666,7 @@
         <v>(True, False, False, True, False, True) : (False, True, False),</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>35</v>
       </c>
@@ -1695,7 +1702,7 @@
         <v>(True, False, False, True, False, False) : (None, None, None),</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -1731,7 +1738,7 @@
         <v>(True, False, False, False, True, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>35</v>
       </c>
@@ -1839,7 +1846,7 @@
         <v>(True, False, False, False, False, False) : (True, True, False),</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>36</v>
       </c>
@@ -1911,7 +1918,7 @@
         <v>(False, True, True, True, True, False) : (False, False, False),</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>36</v>
       </c>
@@ -1947,7 +1954,7 @@
         <v>(False, True, True, True, False, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>36</v>
       </c>
@@ -1983,7 +1990,7 @@
         <v>(False, True, True, True, False, False) : (None, None, None),</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>36</v>
       </c>
@@ -2055,7 +2062,7 @@
         <v>(False, True, True, False, True, False) : (False, False, True),</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>36</v>
       </c>
@@ -2091,7 +2098,7 @@
         <v>(False, True, True, False, False, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>36</v>
       </c>
@@ -2163,7 +2170,7 @@
         <v>(False, True, False, True, True, True) : (False, False, False),</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>36</v>
       </c>
@@ -2199,7 +2206,7 @@
         <v>(False, True, False, True, True, False) : (None, None, None),</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>36</v>
       </c>
@@ -2235,7 +2242,7 @@
         <v>(False, True, False, True, False, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>36</v>
       </c>
@@ -2343,7 +2350,7 @@
         <v>(False, True, False, False, True, False) : (True, False, False),</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>36</v>
       </c>
@@ -2379,7 +2386,7 @@
         <v>(False, True, False, False, False, True) : (None, None, None),</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>36</v>
       </c>
@@ -2415,7 +2422,7 @@
         <v>(False, True, False, False, False, False) : (None, None, None),</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>36</v>
       </c>
@@ -2487,7 +2494,7 @@
         <v>(False, False, True, True, True, False) : (False, True, False),</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>36</v>
       </c>
@@ -2559,7 +2566,7 @@
         <v>(False, False, True, True, False, False) : (False, False, True),</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>36</v>
       </c>
@@ -2631,7 +2638,7 @@
         <v>(False, False, True, False, True, False) : (False, True, True),</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>36</v>
       </c>
@@ -2739,7 +2746,7 @@
         <v>(False, False, False, True, True, True) : (False, True, False),</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>36</v>
       </c>
@@ -2811,7 +2818,7 @@
         <v>(False, False, False, True, False, True) : (False, False, False),</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>36</v>
       </c>
@@ -2992,6 +2999,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K65" xr:uid="{24382A42-B759-4365-AAC8-5AFFA386FC5F}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="False"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="A2:F65">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"True"</formula>

</xml_diff>